<commit_message>
Desenvolvendo o Case do Data Master
</commit_message>
<xml_diff>
--- a/pre_processing/median_training.xlsx
+++ b/pre_processing/median_training.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,67 +468,67 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>plan_list_price</t>
+          <t>payment_plan_days_mov_avg_m3</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>149</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>plan_list_price_mov_avg_m3</t>
+          <t>payment_plan_days_mov_avg_m6</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>149</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>plan_list_price_mov_avg_m6</t>
+          <t>payment_plan_days_mov_max_m3</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>149</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>plan_list_price_max_m3</t>
+          <t>payment_plan_days_mov_max_m6</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>149</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>plan_list_price_max_m6</t>
+          <t>payment_plan_days_mov_min_m3</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>149</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>plan_list_price_min_m3</t>
+          <t>payment_plan_days_mov_min_m6</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>149</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>plan_list_price_min_m6</t>
+          <t>actual_amount_paid</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -538,7 +538,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>actual_amount_paid</t>
+          <t>actual_amount_paid_mov_avg_m3</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -548,7 +548,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>actual_amount_paid_mov_avg_m3</t>
+          <t>actual_amount_paid_mov_avg_m6</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -558,7 +558,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>actual_amount_paid_mov_avg_m6</t>
+          <t>actual_amount_paid_mov_max_m3</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -568,7 +568,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>actual_amount_paid_max_m3</t>
+          <t>actual_amount_paid_mov_max_m6</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -578,7 +578,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>actual_amount_paid_max_m6</t>
+          <t>actual_amount_paid_mov_min_m3</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -588,7 +588,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>actual_amount_paid_min_m3</t>
+          <t>actual_amount_paid_mov_min_m6</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -598,220 +598,510 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>actual_amount_paid_min_m6</t>
+          <t>num_25</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>149</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>num_25</t>
+          <t>num_25_mov_avg_m3</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>57</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>num_50</t>
+          <t>num_25_mov_avg_m6</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>15</v>
+        <v>66.5</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>num_75</t>
+          <t>num_25_mov_max_m3</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>10</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>num_985</t>
+          <t>num_25_mov_max_m6</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>11</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>num_100</t>
+          <t>num_25_mov_min_m3</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>298</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>num_unq</t>
+          <t>num_25_mov_min_m6</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>334</v>
+        <v>66.5</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>num_unq_mov_avg_m3</t>
+          <t>num_50</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>261.3333333333333</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>num_unq_mov_avg_m6</t>
+          <t>num_50_mov_avg_m3</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>273</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>num_unq_max_m3</t>
+          <t>num_50_mov_avg_m6</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>364</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>num_unq_max_m6</t>
+          <t>num_50_mov_max_m3</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>443</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>num_unq_min_m3</t>
+          <t>num_50_mov_max_m6</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>148</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>num_unq_min_m6</t>
+          <t>num_50_mov_min_m3</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>107</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>total_secs</t>
+          <t>num_50_mov_min_m6</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>82250.04399999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>%num_more_than_50</t>
+          <t>num_75</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>79.40000000000001</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>%num_more_than_50_mov_avg_m3</t>
+          <t>num_75_mov_avg_m3</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>76.80333333333334</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>%num_more_than_50_mov_avg_m6</t>
+          <t>num_75_mov_avg_m6</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>76.36999999999999</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>%num_more_than_50_max_m3</t>
+          <t>num_75_mov_max_m3</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>84.14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>%num_more_than_50_max_m6</t>
+          <t>num_75_mov_max_m6</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>86.67</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>%num_more_than_50_min_m3</t>
+          <t>num_75_mov_min_m3</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>70.09999999999999</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>%num_more_than_50_min_m6</t>
+          <t>num_75_mov_min_m6</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>65.75</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
+          <t>num_985</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>num_985_mov_avg_m3</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>11.33333333333333</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>num_985_mov_avg_m6</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>11.66666666666667</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>num_985_mov_max_m3</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>num_985_mov_max_m6</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>num_985_mov_min_m3</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>11.33333333333333</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>num_985_mov_min_m6</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>11.66666666666667</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>num_100</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>num_100_mov_avg_m3</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>315.3333333333333</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>num_100_mov_avg_m6</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>327.1666666666667</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>num_100_mov_max_m3</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>num_100_mov_max_m6</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>num_100_mov_min_m3</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>315.3333333333333</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>num_100_mov_min_m6</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>327.1666666666667</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>num_unq</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>num_unq_mov_avg_m3</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>num_unq_mov_avg_m6</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>361.8333333333333</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>num_unq_mov_max_m3</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>num_unq_mov_max_m6</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>num_unq_mov_min_m3</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>num_unq_mov_min_m6</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>361.8333333333333</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>total_secs</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>82250.04399999999</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>%num_more_than_50</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>79.40000000000001</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>%num_more_than_50_mov_avg_m3</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>78.13000000000001</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>%num_more_than_50_mov_avg_m6</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>77.45999999999999</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>%num_more_than_50_mov_max_m3</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>85.59999999999999</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>%num_more_than_50_mov_max_m6</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>88.37</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>%num_more_than_50_mov_min_m3</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>78.13000000000001</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>%num_more_than_50_mov_min_m6</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>77.45999999999999</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
           <t>months_as_a_registered</t>
         </is>
       </c>
-      <c r="B38" t="n">
+      <c r="B67" t="n">
         <v>30</v>
       </c>
     </row>

</xml_diff>